<commit_message>
Added support for exceptional cases and plan fixing
</commit_message>
<xml_diff>
--- a/4-year-plan-template.xlsx
+++ b/4-year-plan-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nam/Library/CloudStorage/Dropbox/Teaching/effat/admin-stuff/advising-helpers/f25-advising/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nam/Library/CloudStorage/Dropbox/Teaching/effat/admin-stuff/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D302E8AD-2A2F-554F-97B7-AF9000058F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AC2976-D67F-CC43-BAC0-E618F0CD748F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20060" xr2:uid="{9CED95F9-05A7-4F43-87A3-0E2867F21807}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" xr2:uid="{9CED95F9-05A7-4F43-87A3-0E2867F21807}"/>
   </bookViews>
   <sheets>
     <sheet name="Study Plan" sheetId="1" r:id="rId1"/>
@@ -138,9 +138,6 @@
     <t>Principles of Computing, Data and Algorithms</t>
   </si>
   <si>
-    <t>Choice</t>
-  </si>
-  <si>
     <t>English Language II</t>
   </si>
   <si>
@@ -424,9 +421,6 @@
     <t>Equiv</t>
   </si>
   <si>
-    <t>GENG 132</t>
-  </si>
-  <si>
     <t>Foreign 1</t>
   </si>
   <si>
@@ -461,6 +455,12 @@
   </si>
   <si>
     <t>CS4176</t>
+  </si>
+  <si>
+    <t>Science 1</t>
+  </si>
+  <si>
+    <t>English 2</t>
   </si>
 </sst>
 </file>
@@ -1797,8 +1797,8 @@
   </sheetPr>
   <dimension ref="B1:S49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="N42" sqref="N42"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1907,7 +1907,7 @@
       <c r="M4" s="75"/>
       <c r="N4" s="77"/>
       <c r="Q4" s="55" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="S4">
         <f>SUM(F11,M11,F22,M22,F33,M33,F37,F47,M47)</f>
@@ -1978,7 +1978,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H6" s="14">
         <f>IF(COUNTIF(List!$A$4:$A$100,"="&amp;TRIM(B6))=1,1,IF(COUNTIF(List!$F$4:$F$100,"="&amp;TRIM(B6))=1,2,IF(COUNTIF(List!$L$4:$L$100,"="&amp;TRIM(B6))=1,3,0)))</f>
@@ -2032,22 +2032,22 @@
         <v>0</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="J7" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="13">
+        <v>3</v>
+      </c>
+      <c r="L7" s="13">
+        <v>0</v>
+      </c>
+      <c r="M7" s="13">
+        <v>3</v>
+      </c>
+      <c r="N7" s="19" t="s">
         <v>25</v>
-      </c>
-      <c r="K7" s="13">
-        <v>3</v>
-      </c>
-      <c r="L7" s="13">
-        <v>0</v>
-      </c>
-      <c r="M7" s="13">
-        <v>3</v>
-      </c>
-      <c r="N7" s="19" t="s">
-        <v>26</v>
       </c>
       <c r="O7" s="1">
         <f>IF(COUNTIF(List!$A$4:$A$100,"="&amp;TRIM(I7))=1,1,IF(COUNTIF(List!$F$4:$F$100,"="&amp;TRIM(I7))=1,2,IF(COUNTIF(List!$L$4:$L$100,"="&amp;TRIM(I7))=1,3,0)))</f>
@@ -2057,32 +2057,32 @@
     </row>
     <row r="8" spans="2:19" ht="32" x14ac:dyDescent="0.2">
       <c r="B8" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="D8" s="13">
+        <v>3</v>
+      </c>
+      <c r="E8" s="13">
+        <v>0</v>
+      </c>
+      <c r="F8" s="13">
+        <v>3</v>
+      </c>
+      <c r="G8" s="13" t="s">
         <v>27</v>
-      </c>
-      <c r="D8" s="13">
-        <v>3</v>
-      </c>
-      <c r="E8" s="13">
-        <v>0</v>
-      </c>
-      <c r="F8" s="13">
-        <v>3</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>28</v>
       </c>
       <c r="H8" s="14">
         <f>IF(COUNTIF(List!$A$4:$A$100,"="&amp;TRIM(B8))=1,1,IF(COUNTIF(List!$F$4:$F$100,"="&amp;TRIM(B8))=1,2,IF(COUNTIF(List!$L$4:$L$100,"="&amp;TRIM(B8))=1,3,0)))</f>
         <v>0</v>
       </c>
       <c r="I8" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="12" t="s">
         <v>29</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>30</v>
       </c>
       <c r="K8" s="13">
         <v>2</v>
@@ -2104,10 +2104,10 @@
     </row>
     <row r="9" spans="2:19" ht="32" x14ac:dyDescent="0.2">
       <c r="B9" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>31</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>32</v>
       </c>
       <c r="D9" s="13">
         <v>3</v>
@@ -2126,10 +2126,10 @@
         <v>0</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K9" s="13">
         <v>3</v>
@@ -2151,10 +2151,10 @@
     </row>
     <row r="10" spans="2:19" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="13">
         <v>3</v>
@@ -2173,10 +2173,10 @@
         <v>0</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K10" s="13">
         <v>3</v>
@@ -2199,7 +2199,7 @@
     <row r="11" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="22"/>
       <c r="C11" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="24">
         <f>SUM(D5:D10)</f>
@@ -2217,7 +2217,7 @@
       <c r="H11" s="26"/>
       <c r="I11" s="27"/>
       <c r="J11" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K11" s="24">
         <f>SUM(K5:K10)</f>
@@ -2258,7 +2258,7 @@
     </row>
     <row r="13" spans="2:19" ht="25.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="72" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="73"/>
       <c r="D13" s="73"/>
@@ -2275,7 +2275,7 @@
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B14" s="83" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="84"/>
       <c r="D14" s="84"/>
@@ -2284,7 +2284,7 @@
       <c r="G14" s="84"/>
       <c r="H14" s="85"/>
       <c r="I14" s="74" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J14" s="75"/>
       <c r="K14" s="75"/>
@@ -2294,10 +2294,10 @@
     </row>
     <row r="15" spans="2:19" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>39</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>40</v>
       </c>
       <c r="D15" s="13">
         <v>2</v>
@@ -2316,11 +2316,11 @@
         <v>0</v>
       </c>
       <c r="I15" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="J15" s="12" t="s">
-        <v>42</v>
-      </c>
       <c r="K15" s="13">
         <v>2</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>3</v>
       </c>
       <c r="N15" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O15" s="1">
         <f>IF(COUNTIF(List!$A$4:$A$100,"="&amp;TRIM(I15))=1,1,IF(COUNTIF(List!$F$4:$F$100,"="&amp;TRIM(I15))=1,2,IF(COUNTIF(List!$L$4:$L$100,"="&amp;TRIM(I15))=1,3,0)))</f>
@@ -2340,10 +2340,10 @@
     </row>
     <row r="16" spans="2:19" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>43</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>44</v>
       </c>
       <c r="D16" s="13">
         <v>2</v>
@@ -2362,11 +2362,11 @@
         <v>0</v>
       </c>
       <c r="I16" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="J16" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="J16" s="12" t="s">
-        <v>46</v>
-      </c>
       <c r="K16" s="13">
         <v>2</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>3</v>
       </c>
       <c r="N16" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O16" s="1">
         <f>IF(COUNTIF(List!$A$4:$A$100,"="&amp;TRIM(I16))=1,1,IF(COUNTIF(List!$F$4:$F$100,"="&amp;TRIM(I16))=1,2,IF(COUNTIF(List!$L$4:$L$100,"="&amp;TRIM(I16))=1,3,0)))</f>
@@ -2386,10 +2386,10 @@
     </row>
     <row r="17" spans="2:15" ht="32" x14ac:dyDescent="0.2">
       <c r="B17" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="32" t="s">
         <v>47</v>
-      </c>
-      <c r="C17" s="32" t="s">
-        <v>48</v>
       </c>
       <c r="D17" s="33">
         <v>3</v>
@@ -2408,11 +2408,11 @@
         <v>0</v>
       </c>
       <c r="I17" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="J17" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="J17" s="12" t="s">
-        <v>50</v>
-      </c>
       <c r="K17" s="13">
         <v>2</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>3</v>
       </c>
       <c r="N17" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O17" s="1">
         <f>IF(COUNTIF(List!$A$4:$A$100,"="&amp;TRIM(I17))=1,1,IF(COUNTIF(List!$F$4:$F$100,"="&amp;TRIM(I17))=1,2,IF(COUNTIF(List!$L$4:$L$100,"="&amp;TRIM(I17))=1,3,0)))</f>
@@ -2432,10 +2432,10 @@
     </row>
     <row r="18" spans="2:15" ht="32" x14ac:dyDescent="0.2">
       <c r="B18" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>51</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>52</v>
       </c>
       <c r="D18" s="13">
         <v>3</v>
@@ -2454,22 +2454,22 @@
         <v>0</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J18" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="K18" s="13">
+        <v>3</v>
+      </c>
+      <c r="L18" s="13">
+        <v>0</v>
+      </c>
+      <c r="M18" s="13">
+        <v>3</v>
+      </c>
+      <c r="N18" s="19" t="s">
         <v>95</v>
-      </c>
-      <c r="K18" s="13">
-        <v>3</v>
-      </c>
-      <c r="L18" s="13">
-        <v>0</v>
-      </c>
-      <c r="M18" s="13">
-        <v>3</v>
-      </c>
-      <c r="N18" s="19" t="s">
-        <v>96</v>
       </c>
       <c r="O18" s="1">
         <f>IF(COUNTIF(List!$A$4:$A$100,"="&amp;TRIM(I18))=1,1,IF(COUNTIF(List!$F$4:$F$100,"="&amp;TRIM(I18))=1,2,IF(COUNTIF(List!$L$4:$L$100,"="&amp;TRIM(I18))=1,3,0)))</f>
@@ -2478,11 +2478,11 @@
     </row>
     <row r="19" spans="2:15" ht="16" x14ac:dyDescent="0.2">
       <c r="B19" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>54</v>
-      </c>
       <c r="D19" s="13">
         <v>2</v>
       </c>
@@ -2493,17 +2493,17 @@
         <v>3</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H19" s="14">
         <f>IF(COUNTIF(List!$A$4:$A$100,"="&amp;TRIM(B19))=1,1,IF(COUNTIF(List!$F$4:$F$100,"="&amp;TRIM(B19))=1,2,IF(COUNTIF(List!$L$4:$L$100,"="&amp;TRIM(B19))=1,3,0)))</f>
         <v>0</v>
       </c>
       <c r="I19" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="J19" s="12" t="s">
         <v>55</v>
-      </c>
-      <c r="J19" s="12" t="s">
-        <v>56</v>
       </c>
       <c r="K19" s="13">
         <v>2</v>
@@ -2524,10 +2524,10 @@
     </row>
     <row r="20" spans="2:15" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" s="17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" s="13">
         <v>1</v>
@@ -2546,10 +2546,10 @@
         <v>0</v>
       </c>
       <c r="I20" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="J20" s="12" t="s">
         <v>58</v>
-      </c>
-      <c r="J20" s="12" t="s">
-        <v>59</v>
       </c>
       <c r="K20" s="13">
         <v>1</v>
@@ -2561,7 +2561,7 @@
         <v>2</v>
       </c>
       <c r="N20" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O20" s="1">
         <f>IF(COUNTIF(List!$A$4:$A$100,"="&amp;TRIM(I20))=1,1,IF(COUNTIF(List!$F$4:$F$100,"="&amp;TRIM(I20))=1,2,IF(COUNTIF(List!$L$4:$L$100,"="&amp;TRIM(I20))=1,3,0)))</f>
@@ -2570,10 +2570,10 @@
     </row>
     <row r="21" spans="2:15" ht="32" x14ac:dyDescent="0.2">
       <c r="B21" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>61</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>62</v>
       </c>
       <c r="D21" s="20">
         <v>2</v>
@@ -2592,10 +2592,10 @@
         <v>0</v>
       </c>
       <c r="I21" s="17" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K21" s="13">
         <v>1</v>
@@ -2617,7 +2617,7 @@
     <row r="22" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="22"/>
       <c r="C22" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22" s="24">
         <f>SUM(D15:D21)</f>
@@ -2635,7 +2635,7 @@
       <c r="H22" s="26"/>
       <c r="I22" s="27"/>
       <c r="J22" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K22" s="24">
         <f>SUM(K15:K21)</f>
@@ -2674,7 +2674,7 @@
     </row>
     <row r="24" spans="2:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="72" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C24" s="73"/>
       <c r="D24" s="73"/>
@@ -2691,7 +2691,7 @@
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B25" s="86" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C25" s="87"/>
       <c r="D25" s="87"/>
@@ -2700,7 +2700,7 @@
       <c r="G25" s="87"/>
       <c r="H25" s="88"/>
       <c r="I25" s="68" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J25" s="69"/>
       <c r="K25" s="69"/>
@@ -2710,10 +2710,10 @@
     </row>
     <row r="26" spans="2:15" ht="16" x14ac:dyDescent="0.2">
       <c r="B26" s="15" t="s">
-        <v>24</v>
+        <v>130</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D26" s="13">
         <v>2</v>
@@ -2725,17 +2725,17 @@
         <v>3</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H26" s="14">
         <f>IF(COUNTIF(List!$A$4:$A$100,"="&amp;TRIM(B26))=1,1,IF(COUNTIF(List!$F$4:$F$100,"="&amp;TRIM(B26))=1,2,IF(COUNTIF(List!$L$4:$L$100,"="&amp;TRIM(B26))=1,3,0)))</f>
         <v>0</v>
       </c>
       <c r="I26" s="17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K26" s="13">
         <v>3</v>
@@ -2754,11 +2754,11 @@
     </row>
     <row r="27" spans="2:15" ht="16" x14ac:dyDescent="0.2">
       <c r="B27" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="12" t="s">
-        <v>68</v>
-      </c>
       <c r="D27" s="13">
         <v>3</v>
       </c>
@@ -2769,18 +2769,18 @@
         <v>3</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H27" s="14">
         <f>IF(COUNTIF(List!$A$4:$A$100,"="&amp;TRIM(B27))=1,1,IF(COUNTIF(List!$F$4:$F$100,"="&amp;TRIM(B27))=1,2,IF(COUNTIF(List!$L$4:$L$100,"="&amp;TRIM(B27))=1,3,0)))</f>
         <v>0</v>
       </c>
       <c r="I27" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="J27" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="J27" s="12" t="s">
-        <v>72</v>
-      </c>
       <c r="K27" s="13">
         <v>3</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>3</v>
       </c>
       <c r="N27" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O27" s="1">
         <f>IF(COUNTIF(List!$A$4:$A$100,"="&amp;TRIM(I27))=1,1,IF(COUNTIF(List!$F$4:$F$100,"="&amp;TRIM(I27))=1,2,IF(COUNTIF(List!$L$4:$L$100,"="&amp;TRIM(I27))=1,3,0)))</f>
@@ -2800,11 +2800,11 @@
     </row>
     <row r="28" spans="2:15" ht="16" x14ac:dyDescent="0.2">
       <c r="B28" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="D28" s="13">
         <v>2</v>
       </c>
@@ -2815,29 +2815,29 @@
         <v>3</v>
       </c>
       <c r="G28" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H28" s="14">
         <f>IF(COUNTIF(List!$A$4:$A$100,"="&amp;TRIM(B28))=1,1,IF(COUNTIF(List!$F$4:$F$100,"="&amp;TRIM(B28))=1,2,IF(COUNTIF(List!$L$4:$L$100,"="&amp;TRIM(B28))=1,3,0)))</f>
         <v>0</v>
       </c>
       <c r="I28" s="35" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J28" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="K28" s="36">
+        <v>2</v>
+      </c>
+      <c r="L28" s="36">
+        <v>2</v>
+      </c>
+      <c r="M28" s="36">
+        <v>3</v>
+      </c>
+      <c r="N28" s="19" t="s">
         <v>75</v>
-      </c>
-      <c r="K28" s="36">
-        <v>2</v>
-      </c>
-      <c r="L28" s="36">
-        <v>2</v>
-      </c>
-      <c r="M28" s="36">
-        <v>3</v>
-      </c>
-      <c r="N28" s="19" t="s">
-        <v>76</v>
       </c>
       <c r="O28" s="1">
         <f>IF(COUNTIF(List!$A$4:$A$100,"="&amp;TRIM(I28))=1,1,IF(COUNTIF(List!$F$4:$F$100,"="&amp;TRIM(I28))=1,2,IF(COUNTIF(List!$L$4:$L$100,"="&amp;TRIM(I28))=1,3,0)))</f>
@@ -2846,11 +2846,11 @@
     </row>
     <row r="29" spans="2:15" ht="16" x14ac:dyDescent="0.2">
       <c r="B29" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>74</v>
-      </c>
       <c r="D29" s="13">
         <v>2</v>
       </c>
@@ -2861,17 +2861,17 @@
         <v>3</v>
       </c>
       <c r="G29" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H29" s="14">
         <f>IF(COUNTIF(List!$A$4:$A$100,"="&amp;TRIM(B29))=1,1,IF(COUNTIF(List!$F$4:$F$100,"="&amp;TRIM(B29))=1,2,IF(COUNTIF(List!$L$4:$L$100,"="&amp;TRIM(B29))=1,3,0)))</f>
         <v>0</v>
       </c>
       <c r="I29" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J29" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K29" s="20">
         <v>2</v>
@@ -2883,7 +2883,7 @@
         <v>2</v>
       </c>
       <c r="N29" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O29" s="1">
         <f>IF(COUNTIF(List!$A$4:$A$100,"="&amp;TRIM(I29))=1,1,IF(COUNTIF(List!$F$4:$F$100,"="&amp;TRIM(I29))=1,2,IF(COUNTIF(List!$L$4:$L$100,"="&amp;TRIM(I29))=1,3,0)))</f>
@@ -2892,10 +2892,10 @@
     </row>
     <row r="30" spans="2:15" ht="16" x14ac:dyDescent="0.2">
       <c r="B30" s="17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D30" s="20">
         <v>2</v>
@@ -2912,10 +2912,10 @@
         <v>0</v>
       </c>
       <c r="I30" s="17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J30" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K30" s="20">
         <v>2</v>
@@ -2934,11 +2934,11 @@
     </row>
     <row r="31" spans="2:15" ht="32" x14ac:dyDescent="0.2">
       <c r="B31" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>79</v>
-      </c>
       <c r="D31" s="13">
         <v>3</v>
       </c>
@@ -2949,17 +2949,17 @@
         <v>3</v>
       </c>
       <c r="G31" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H31" s="14">
         <f>IF(COUNTIF(List!$A$4:$A$100,"="&amp;TRIM(B31))=1,1,IF(COUNTIF(List!$F$4:$F$100,"="&amp;TRIM(B31))=1,2,IF(COUNTIF(List!$L$4:$L$100,"="&amp;TRIM(B31))=1,3,0)))</f>
         <v>0</v>
       </c>
       <c r="I31" s="17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J31" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K31" s="20">
         <v>2</v>
@@ -3001,7 +3001,7 @@
     <row r="33" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="38"/>
       <c r="C33" s="39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D33" s="24">
         <f>SUM(D26:D32)</f>
@@ -3019,7 +3019,7 @@
       <c r="H33" s="41"/>
       <c r="I33" s="27"/>
       <c r="J33" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K33" s="24">
         <f>SUM(K26:K32)</f>
@@ -3058,7 +3058,7 @@
     </row>
     <row r="35" spans="2:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B35" s="72" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C35" s="73"/>
       <c r="D35" s="73"/>
@@ -3075,11 +3075,11 @@
     </row>
     <row r="36" spans="2:15" ht="16" x14ac:dyDescent="0.2">
       <c r="B36" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="44" t="s">
-        <v>105</v>
-      </c>
       <c r="D36" s="45">
         <v>0</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>3</v>
       </c>
       <c r="G36" s="46" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H36" s="14">
         <f>IF(COUNTIF(List!$A$4:$A$100,"="&amp;TRIM(B36))=1,1,IF(COUNTIF(List!$F$4:$F$100,"="&amp;TRIM(B36))=1,2,IF(COUNTIF(List!$L$4:$L$100,"="&amp;TRIM(B36))=1,3,0)))</f>
@@ -3106,7 +3106,7 @@
     <row r="37" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B37" s="38"/>
       <c r="C37" s="39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D37" s="24">
         <f>SUM(D36:D36)</f>
@@ -3145,7 +3145,7 @@
     </row>
     <row r="39" spans="2:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B39" s="79" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C39" s="80"/>
       <c r="D39" s="80"/>
@@ -3162,7 +3162,7 @@
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B40" s="65" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C40" s="66"/>
       <c r="D40" s="66"/>
@@ -3171,7 +3171,7 @@
       <c r="G40" s="67"/>
       <c r="H40" s="49"/>
       <c r="I40" s="68" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J40" s="69"/>
       <c r="K40" s="69"/>
@@ -3182,10 +3182,10 @@
     </row>
     <row r="41" spans="2:15" ht="16" x14ac:dyDescent="0.2">
       <c r="B41" s="93" t="s">
+        <v>105</v>
+      </c>
+      <c r="C41" s="96" t="s">
         <v>106</v>
-      </c>
-      <c r="C41" s="96" t="s">
-        <v>107</v>
       </c>
       <c r="D41" s="96">
         <v>0</v>
@@ -3197,17 +3197,17 @@
         <v>6</v>
       </c>
       <c r="G41" s="99" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H41" s="14">
         <f>IF(COUNTIF(List!$A$4:$A$100,"="&amp;TRIM(B41))=1,1,IF(COUNTIF(List!$F$4:$F$100,"="&amp;TRIM(B41))=1,2,IF(COUNTIF(List!$L$4:$L$100,"="&amp;TRIM(B41))=1,3,0)))</f>
         <v>0</v>
       </c>
       <c r="I41" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J41" s="50" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K41" s="51">
         <v>0</v>
@@ -3219,7 +3219,7 @@
         <v>2</v>
       </c>
       <c r="N41" s="19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="O41" s="1">
         <f>IF(COUNTIF(List!$A$4:$A$100,"="&amp;TRIM(I41))=1,1,IF(COUNTIF(List!$F$4:$F$100,"="&amp;TRIM(I41))=1,2,IF(COUNTIF(List!$L$4:$L$100,"="&amp;TRIM(I41))=1,3,0)))</f>
@@ -3235,11 +3235,11 @@
       <c r="G42" s="100"/>
       <c r="H42" s="52"/>
       <c r="I42" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="J42" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="J42" s="21" t="s">
-        <v>87</v>
-      </c>
       <c r="K42" s="13">
         <v>2</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>3</v>
       </c>
       <c r="N42" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O42" s="1">
         <f>IF(COUNTIF(List!$A$4:$A$100,"="&amp;TRIM(I42))=1,1,IF(COUNTIF(List!$F$4:$F$100,"="&amp;TRIM(I42))=1,2,IF(COUNTIF(List!$L$4:$L$100,"="&amp;TRIM(I42))=1,3,0)))</f>
@@ -3266,11 +3266,11 @@
       <c r="G43" s="100"/>
       <c r="H43" s="52"/>
       <c r="I43" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="J43" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="J43" s="12" t="s">
-        <v>89</v>
-      </c>
       <c r="K43" s="13">
         <v>3</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>3</v>
       </c>
       <c r="N43" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O43" s="1">
         <f>IF(COUNTIF(List!$A$4:$A$100,"="&amp;TRIM(I43))=1,1,IF(COUNTIF(List!$F$4:$F$100,"="&amp;TRIM(I43))=1,2,IF(COUNTIF(List!$L$4:$L$100,"="&amp;TRIM(I43))=1,3,0)))</f>
@@ -3297,10 +3297,10 @@
       <c r="G44" s="100"/>
       <c r="H44" s="52"/>
       <c r="I44" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="J44" s="12" t="s">
         <v>90</v>
-      </c>
-      <c r="J44" s="12" t="s">
-        <v>91</v>
       </c>
       <c r="K44" s="13">
         <v>2</v>
@@ -3328,10 +3328,10 @@
       <c r="G45" s="100"/>
       <c r="H45" s="52"/>
       <c r="I45" s="17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J45" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K45" s="20">
         <v>2</v>
@@ -3357,10 +3357,10 @@
       <c r="G46" s="101"/>
       <c r="H46" s="54"/>
       <c r="I46" s="17" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J46" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K46" s="51">
         <v>2</v>
@@ -3380,7 +3380,7 @@
     <row r="47" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B47" s="27"/>
       <c r="C47" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D47" s="24">
         <f>SUM(D40:D46)</f>
@@ -3398,7 +3398,7 @@
       <c r="H47" s="26"/>
       <c r="I47" s="27"/>
       <c r="J47" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K47" s="24">
         <f>SUM(K40:K46)</f>
@@ -3438,7 +3438,7 @@
     </row>
     <row r="49" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B49" s="89" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C49" s="90"/>
       <c r="D49" s="91">
@@ -3520,28 +3520,28 @@
   <sheetData>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="60" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B3" s="61" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3" s="61" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D3" s="61"/>
       <c r="E3" s="61"/>
       <c r="F3" s="62" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G3" s="61" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H3" s="61"/>
       <c r="I3" s="61"/>
       <c r="J3" s="63"/>
       <c r="K3" s="63"/>
       <c r="L3" s="64" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>